<commit_message>
small update after check
</commit_message>
<xml_diff>
--- a/Names_borg_d.xlsx
+++ b/Names_borg_d.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\R\fuortesa\dynamic-era-energy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\R\quikj\SimpleBox_work\dynamic-era-energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4C733C-4579-4057-9ECA-6172E6273BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01306C59-EACA-4CB5-814D-4C64EF643D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="oldlvl" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="145">
   <si>
     <t>old.lvl</t>
   </si>
@@ -807,582 +807,582 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="3"/>
+    <col min="1" max="1" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>114</v>
       </c>
@@ -1395,18 +1395,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4642A90-48BA-45EF-91C6-C0D999F1DDB8}">
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>121</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>132</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>116</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>137</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>138</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>139</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>144</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>142</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>143</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>119</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>117</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>118</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>119</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>117</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>118</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>119</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>117</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>118</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>119</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>117</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>118</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>119</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>118</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>119</v>
       </c>
@@ -1758,571 +1758,563 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="B50" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B53" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B57" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B60" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B66" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B73" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B80" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B87" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B94" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B98" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B102" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B109" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B112" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B115" s="1" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>